<commit_message>
Fixed data issues: 2008 silver spotted sculpin measured 335 mm -> tally 1 with note of length; 2018 typo PSL length 45120 mm -> seperate 45 & 120 mm obs; 2018 capelin length 1000 mm -> count 1000 & no lengths.
</commit_message>
<xml_diff>
--- a/noaa-nfa/FishAtlas_2008-kbnerr_sub.2022.04.02.xlsx
+++ b/noaa-nfa/FishAtlas_2008-kbnerr_sub.2022.04.02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chguo/nearshore-fish/noaa-nfa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9473407-720C-9C4E-BDE0-E4B21EE048C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE05A673-3F91-1543-90EB-EE9A05775FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32920" yWindow="-9440" windowWidth="22960" windowHeight="17500" activeTab="3" xr2:uid="{3B314B78-36D3-428A-9610-1FB3858E89CC}"/>
   </bookViews>
@@ -915,7 +915,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="88">
   <si>
     <t>SiteID</t>
   </si>
@@ -1176,6 +1176,9 @@
   </si>
   <si>
     <t>Homer Spit</t>
+  </si>
+  <si>
+    <t>Noted length 335 mm - likely typo, changed NFA sub to 1 unmeasured.</t>
   </si>
 </sst>
 </file>
@@ -2030,8 +2033,8 @@
   <dimension ref="A1:K656"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A618" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F651" sqref="F651"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2281,13 +2284,10 @@
         <v>37</v>
       </c>
       <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>335</v>
-      </c>
-      <c r="J10" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>